<commit_message>
calc compress ratio for k-means
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smallcat\Documents\github\data-compression\impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyao\Documents\GitHub\data-compression\impl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16836" yWindow="9264" windowWidth="28980" windowHeight="16140" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="16840" yWindow="9260" windowWidth="28980" windowHeight="16140" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -182,12 +182,16 @@
     <t>execution time (iteration = 1000, clusters = 1000)</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>compress ratio (iteration = 1000, clusters = 1000)</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1781,7 +1785,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2169,7 +2172,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2281,7 +2283,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2667,7 +2668,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2749,7 +2749,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2850,7 +2849,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3257,7 +3255,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7974,12 +7971,12 @@
       <selection activeCell="B20" sqref="B20:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.69921875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8005,7 +8002,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8031,7 +8028,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -8060,7 +8057,7 @@
         <v>3.96469</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -8089,7 +8086,7 @@
         <v>15.012912</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -8118,7 +8115,7 @@
         <v>3.8102360000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -8138,7 +8135,7 @@
         <v>12.947824000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -8146,7 +8143,7 @@
         <v>3.7763</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -8154,7 +8151,7 @@
         <v>10.402900000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -8162,7 +8159,7 @@
         <v>2.8954</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -8170,7 +8167,7 @@
         <v>5.4892000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -8178,7 +8175,7 @@
         <v>1.0692999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -8186,12 +8183,12 @@
         <v>0.98680000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -8208,7 +8205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>50.246116000000001</v>
       </c>
@@ -8222,12 +8219,12 @@
         <v>57.471921000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -8244,7 +8241,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>8.1706539999999999E-4</v>
       </c>
@@ -8274,17 +8271,17 @@
       <selection activeCell="A11" sqref="A11:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -8304,7 +8301,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -8324,7 +8321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -8344,7 +8341,7 @@
         <v>2.1447829999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -8352,7 +8349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -8393,7 +8390,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -8431,7 +8428,7 @@
         <v>4.2465000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -8451,12 +8448,12 @@
         <v>2.826E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -8476,12 +8473,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -8511,20 +8508,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -8547,7 +8544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3.6736149999999999</v>
       </c>
@@ -8567,12 +8564,12 @@
         <v>3.8312430000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -8592,7 +8589,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -8612,12 +8609,12 @@
         <v>3.86E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -8640,7 +8637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>37.079129000000002</v>
       </c>
@@ -8660,12 +8657,12 @@
         <v>35.168976999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -8685,7 +8682,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -8703,10 +8700,60 @@
       </c>
       <c r="F15">
         <v>4.2000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C19">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D19">
+        <v>1E-4</v>
+      </c>
+      <c r="E19">
+        <v>1E-3</v>
+      </c>
+      <c r="F19">
+        <v>0.01</v>
+      </c>
+      <c r="G19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f xml:space="preserve"> 1/0.979871</f>
+        <v>1.0205424999821404</v>
+      </c>
+      <c r="C20">
+        <v>1.019641</v>
+      </c>
+      <c r="D20">
+        <v>1.036257</v>
+      </c>
+      <c r="E20">
+        <v>1.059337</v>
+      </c>
+      <c r="F20">
+        <v>1.156326</v>
+      </c>
+      <c r="G20">
+        <v>1.359143</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compress time / total time
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyao\Documents\GitHub\data-compression\impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE84B12-8561-D547-AA47-DA4BB4EE4149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="1940" windowWidth="28980" windowHeight="16140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6860" yWindow="1940" windowWidth="28980" windowHeight="16140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
@@ -17,11 +18,12 @@
     <sheet name="k-means" sheetId="3" r:id="rId3"/>
     <sheet name="fftss" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -224,12 +226,20 @@
     <t>c-16</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>compress_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>total_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -677,7 +687,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1129,7 +1138,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1219,7 +1227,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1633,7 +1640,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2081,7 +2087,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5597,7 +5602,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6051,7 +6055,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13911,7 +13914,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="グラフ 4"/>
+        <xdr:cNvPr id="5" name="グラフ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -13941,7 +13950,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="グラフ 5"/>
+        <xdr:cNvPr id="6" name="グラフ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -14262,19 +14277,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -14300,7 +14315,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -14326,7 +14341,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -14355,7 +14370,7 @@
         <v>3.96469</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -14384,7 +14399,7 @@
         <v>15.012912</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -14413,7 +14428,7 @@
         <v>3.8102360000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="E6" t="s">
         <v>20</v>
       </c>
@@ -14433,7 +14448,7 @@
         <v>12.947824000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -14441,7 +14456,7 @@
         <v>3.7763</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -14449,7 +14464,7 @@
         <v>10.402900000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -14457,7 +14472,7 @@
         <v>2.8954</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -14465,7 +14480,7 @@
         <v>5.4892000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -14473,7 +14488,7 @@
         <v>1.0692999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -14481,12 +14496,12 @@
         <v>0.98680000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -14503,7 +14518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16">
         <v>50.246116000000001</v>
       </c>
@@ -14517,12 +14532,12 @@
         <v>57.471921000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -14539,7 +14554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="B21" s="1">
         <v>8.1706539999999999E-4</v>
       </c>
@@ -14562,24 +14577,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -14599,7 +14614,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -14619,7 +14634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -14639,7 +14654,7 @@
         <v>2.1447829999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -14647,7 +14662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -14688,7 +14703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -14726,7 +14741,7 @@
         <v>4.2465000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -14746,12 +14761,12 @@
         <v>2.826E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -14771,12 +14786,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -14805,21 +14820,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -14842,7 +14857,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="B3">
         <v>3.6736149999999999</v>
       </c>
@@ -14862,12 +14877,12 @@
         <v>3.8312430000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -14887,7 +14902,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -14907,12 +14922,12 @@
         <v>3.86E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -14935,7 +14950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="B11">
         <v>37.079129000000002</v>
       </c>
@@ -14955,12 +14970,12 @@
         <v>35.168976999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -14980,7 +14995,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -15000,12 +15015,12 @@
         <v>4.2000000000000002E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -15028,7 +15043,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <f xml:space="preserve"> 1/0.979871</f>
         <v>1.0205424999821404</v>
@@ -15049,12 +15064,12 @@
         <v>1.359143</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -15077,7 +15092,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>596.92707900000005</v>
       </c>
@@ -15097,12 +15112,12 @@
         <v>602.11321499999997</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -15125,7 +15140,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -15148,12 +15163,12 @@
         <v>1.042E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -15176,7 +15191,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7">
       <c r="B33">
         <v>2.4117739999999999</v>
       </c>
@@ -15205,21 +15220,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -15239,7 +15254,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="B3">
         <f>AVERAGE(B4:B7)</f>
         <v>6.21041825</v>
@@ -15261,7 +15276,7 @@
         <v>6.21041825</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="B4">
         <v>7.9996809999999998</v>
       </c>
@@ -15278,7 +15293,7 @@
         <v>7.9996809999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="B5">
         <v>7.9996809999999998</v>
       </c>
@@ -15295,7 +15310,7 @@
         <v>7.9996809999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="B6">
         <v>1.0025649999999999</v>
       </c>
@@ -15312,7 +15327,7 @@
         <v>1.0025649999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="B7">
         <v>7.8397459999999999</v>
       </c>
@@ -15329,12 +15344,12 @@
         <v>7.8397459999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -15357,7 +15372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="B11">
         <v>4.2609000000000001E-2</v>
       </c>
@@ -15377,7 +15392,7 @@
         <v>0.26097100000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -15394,7 +15409,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="B13">
         <v>4.2609000000000001E-2</v>
       </c>
@@ -15409,6 +15424,56 @@
       </c>
       <c r="F13">
         <v>1.553126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15">
+        <v>2.2270000000000002E-2</v>
+      </c>
+      <c r="E15">
+        <v>2.8202000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="D16">
+        <v>1.9782000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>2.2936000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17">
+        <v>1.8460000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>2.4346E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18">
+        <v>2.6015E-2</v>
+      </c>
+      <c r="E18">
+        <v>3.0252999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19">
+        <f>SUM(D15:D18)</f>
+        <v>8.6527000000000007E-2</v>
+      </c>
+      <c r="E19">
+        <f>SUM(E15:E18)</f>
+        <v>0.105737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revise mycompress for himeno
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC65BBA-5E69-D148-B9DC-9C016A6D1D24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D914FCA9-97D4-C344-8159-CB6CEBCFAFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="720" windowWidth="28980" windowHeight="18400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2440" windowWidth="28980" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -250,12 +250,24 @@
     <t>compressed (sz-mod, double)</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>sz-mod-0.0001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sz-mod-0.001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sz-mod-0.01</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +296,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -318,9 +338,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -14594,16 +14615,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>341502</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>45455</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>862202</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>185155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>759543</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>121656</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>302343</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>70856</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14630,16 +14651,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>622026</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>545826</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>305621</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>70718</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>229421</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19918</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14666,16 +14687,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15385,8 +15406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E21"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
@@ -15622,6 +15643,15 @@
       <c r="E15" t="s">
         <v>27</v>
       </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16">
@@ -15637,12 +15667,32 @@
         <v>57.471921000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="17" spans="1:8">
+      <c r="B17">
+        <v>59.392279000000002</v>
+      </c>
+      <c r="D17">
+        <v>62.361249999999998</v>
+      </c>
+      <c r="E17">
+        <v>59.768925000000003</v>
+      </c>
+      <c r="F17">
+        <v>59.029927999999998</v>
+      </c>
+      <c r="G17">
+        <v>60.659789000000004</v>
+      </c>
+      <c r="H17">
+        <v>61.856563999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -15659,7 +15709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:8">
       <c r="B21" s="1">
         <v>8.1706539999999999E-4</v>
       </c>
@@ -15685,7 +15735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cpu time for himeno
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D914FCA9-97D4-C344-8159-CB6CEBCFAFFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC5610-7AE2-7647-BCCF-B1E715BCA391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2440" windowWidth="28980" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="1780" windowWidth="28980" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -128,10 +128,6 @@
   </si>
   <si>
     <t>sz-mod-0.00001</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sz-mod-0.0000001</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -719,456 +715,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>compress ratio (iteration = 1000, clusters = 1000)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'k-means'!$A$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'k-means'!$B$19:$G$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.9999999999999995E-7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0000000000000001E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'k-means'!$B$20:$G$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.0205424999821404</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.019641</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.036257</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.059337</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.156326</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.359143</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-863B-409E-8C94-8FE1399EAFA9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1138082288"/>
-        <c:axId val="1138082704"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1138082288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP"/>
-                  <a:t>absErrBound</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.44020713035870518"/>
-              <c:y val="0.90182852143482062"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1138082704"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1138082704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP"/>
-                  <a:t>Compression ratio</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="8.3333333333333332E-3"/>
-              <c:y val="0.29895049577136196"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1138082288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ja-JP"/>
               <a:t>Gosa (65536 data, deviation from means)</a:t>
             </a:r>
             <a:endParaRPr lang="ja-JP" altLang="en-US"/>
@@ -1636,7 +1182,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -2084,7 +1630,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -2529,7 +2075,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -3705,442 +3251,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ja-JP"/>
-              <a:t>CPU Time</a:t>
-            </a:r>
-            <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>himeno!$B$15:$E$15</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>uncompressed</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>sz-mod-0.0000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>sz-mod-0.000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>sz-mod-0.00001</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>himeno!$B$16:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>50.246116000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55.305459999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>52.922677999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>57.471921000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-22AB-4B81-848B-7D9B18E0BD41}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1279226655"/>
-        <c:axId val="1279234143"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1279226655"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>absErrBound</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.43705424321959757"/>
-              <c:y val="0.90182852143482062"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1279234143"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1279234143"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP"/>
-                  <a:t>cpu</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" baseline="0"/>
-                  <a:t> time (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="8.3333333333333332E-3"/>
-              <c:y val="0.37302456984543603"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="ja-JP"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ja-JP"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1279226655"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ja-JP"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ja-JP"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="ja-JP"/>
               <a:t>compression ratio</a:t>
             </a:r>
             <a:endParaRPr lang="ja-JP" altLang="en-US"/>
@@ -4678,7 +3788,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -5174,7 +4284,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -5655,7 +4765,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -6109,7 +5219,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -6562,7 +5672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -7009,6 +6119,456 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>compress ratio (iteration = 1000, clusters = 1000)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'k-means'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'k-means'!$B$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'k-means'!$B$20:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0205424999821404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.019641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.036257</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.059337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.156326</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.359143</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-863B-409E-8C94-8FE1399EAFA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1138082288"/>
+        <c:axId val="1138082704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1138082288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>absErrBound</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44020713035870518"/>
+              <c:y val="0.90182852143482062"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1138082704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1138082704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ja-JP"/>
+                  <a:t>Compression ratio</a:t>
+                </a:r>
+                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.3333333333333332E-3"/>
+              <c:y val="0.29895049577136196"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1138082288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7170,46 +6730,6 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10084,8 +9604,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10587,8 +10107,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -11090,7 +10610,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11593,7 +11113,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12096,7 +11616,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12599,7 +12119,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13102,7 +12622,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13605,7 +13125,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14108,523 +13628,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>862202</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>185155</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>608202</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>58155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>302343</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>70856</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>429343</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>134356</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14651,16 +13668,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>545826</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406126</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>229421</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19918</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>89721</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>108818</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14680,42 +13697,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -15407,7 +14388,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A15" sqref="A15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
@@ -15641,58 +14622,41 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16">
-        <v>50.246116000000001</v>
+        <v>59.392279000000002</v>
       </c>
       <c r="C16">
-        <v>55.305459999999997</v>
+        <v>60.581772000000001</v>
       </c>
       <c r="D16">
-        <v>52.922677999999998</v>
+        <v>59.844496999999997</v>
       </c>
       <c r="E16">
-        <v>57.471921000000002</v>
+        <v>60.232497000000002</v>
+      </c>
+      <c r="F16">
+        <v>59.970162000000002</v>
+      </c>
+      <c r="G16">
+        <v>60.722251999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="B17">
-        <v>59.392279000000002</v>
-      </c>
-      <c r="D17">
-        <v>62.361249999999998</v>
-      </c>
-      <c r="E17">
-        <v>59.768925000000003</v>
-      </c>
-      <c r="F17">
-        <v>59.029927999999998</v>
-      </c>
-      <c r="G17">
-        <v>60.659789000000004</v>
-      </c>
-      <c r="H17">
-        <v>61.856563999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -15709,7 +14673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:5">
       <c r="B21" s="1">
         <v>8.1706539999999999E-4</v>
       </c>
@@ -15791,7 +14755,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>1.0841719999999999</v>
@@ -15811,7 +14775,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>1.0995969999999999</v>
@@ -15831,10 +14795,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
         <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -15860,22 +14824,22 @@
         <v>14</v>
       </c>
       <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>29</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>30</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>31</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>32</v>
-      </c>
-      <c r="N7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -16006,7 +14970,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -16014,22 +14978,22 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -16099,7 +15063,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -16107,22 +15071,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -16192,7 +15156,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -16241,7 +15205,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -16249,22 +15213,22 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>30</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>31</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>32</v>
-      </c>
-      <c r="G23" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -16340,7 +15304,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -16406,7 +15370,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -16521,7 +15485,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -16529,22 +15493,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -16569,19 +15533,19 @@
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -16603,10 +15567,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
         <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -16657,12 +15621,12 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>4.2609000000000001E-2</v>
@@ -16670,7 +15634,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22">
         <v>0.21291599999999999</v>
@@ -16678,7 +15642,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>3.8682000000000001E-2</v>

</xml_diff>

<commit_message>
add result for test
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC5610-7AE2-7647-BCCF-B1E715BCA391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA6EF95-24EC-6244-A4AF-04E002CBE2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="1780" windowWidth="28980" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="3960" windowWidth="28980" windowHeight="18400" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
     <sheet name="ping-pong" sheetId="2" r:id="rId2"/>
     <sheet name="k-means" sheetId="3" r:id="rId3"/>
-    <sheet name="fftss" sheetId="4" r:id="rId4"/>
+    <sheet name="k-means(test)" sheetId="5" r:id="rId4"/>
+    <sheet name="k-means(obs_info)" sheetId="6" r:id="rId5"/>
+    <sheet name="fftss" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -256,6 +258,14 @@
   </si>
   <si>
     <t>sz-mod-0.01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>execution time (100000, iteration = 1000, clusters = 100)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>execution time (100000, iteration = 1000, clusters = 1000)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -14387,7 +14397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:G16"/>
     </sheetView>
   </sheetViews>
@@ -14962,8 +14972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -15359,6 +15369,498 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F16A6CE-46E7-D546-BCF2-FDFB0D886630}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <v>17.508977999999999</v>
+      </c>
+      <c r="C3">
+        <v>18.051579</v>
+      </c>
+      <c r="D3">
+        <v>18.916996000000001</v>
+      </c>
+      <c r="E3">
+        <v>18.005952000000001</v>
+      </c>
+      <c r="F3">
+        <v>18.438917</v>
+      </c>
+      <c r="G3">
+        <v>17.999881999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D6">
+        <v>1E-4</v>
+      </c>
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D7">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="E7">
+        <v>7.7999999999999999E-5</v>
+      </c>
+      <c r="F7">
+        <v>7.7999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12">
+        <v>1.1000529999999999</v>
+      </c>
+      <c r="C12">
+        <v>1.676909</v>
+      </c>
+      <c r="D12">
+        <v>2.7701730000000002</v>
+      </c>
+      <c r="E12">
+        <v>6.6116710000000003</v>
+      </c>
+      <c r="F12">
+        <v>6.6116710000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17">
+        <v>167.09126599999999</v>
+      </c>
+      <c r="C17">
+        <v>171.21648300000001</v>
+      </c>
+      <c r="D17">
+        <v>167.42308499999999</v>
+      </c>
+      <c r="E17">
+        <v>166.890038</v>
+      </c>
+      <c r="F17">
+        <v>169.91999300000001</v>
+      </c>
+      <c r="G17">
+        <v>166.793948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D20">
+        <v>1E-4</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20">
+        <v>0.01</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D21">
+        <v>4.0900000000000002E-4</v>
+      </c>
+      <c r="E21">
+        <v>3.7599999999999998E-4</v>
+      </c>
+      <c r="F21">
+        <v>3.7599999999999998E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D25">
+        <v>1E-4</v>
+      </c>
+      <c r="E25">
+        <v>1E-3</v>
+      </c>
+      <c r="F25">
+        <v>0.01</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26">
+        <v>1.5219180000000001</v>
+      </c>
+      <c r="C26">
+        <v>3.7388219999999999</v>
+      </c>
+      <c r="D26">
+        <v>6.6444130000000001</v>
+      </c>
+      <c r="E26">
+        <v>7.835483</v>
+      </c>
+      <c r="F26">
+        <v>7.835483</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D4BC53-861A-4F44-A625-5CE21B6F2D0F}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D6">
+        <v>1E-4</v>
+      </c>
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D20">
+        <v>1E-4</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20">
+        <v>0.01</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D25">
+        <v>1E-4</v>
+      </c>
+      <c r="E25">
+        <v>1E-3</v>
+      </c>
+      <c r="F25">
+        <v>0.01</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>

</xml_diff>

<commit_message>
results for obs_info & num_plasma on calc4
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738A06A8-55A6-514A-A58A-5687AAD8B5D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9364D92A-5F5A-1A41-B676-3F6E13D97A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="3960" windowWidth="28980" windowHeight="18400" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4200" windowWidth="28980" windowHeight="18400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="himeno" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="k-means" sheetId="3" r:id="rId3"/>
     <sheet name="k-means(test)" sheetId="5" r:id="rId4"/>
     <sheet name="k-means(obs_info)" sheetId="6" r:id="rId5"/>
-    <sheet name="fftss" sheetId="4" r:id="rId6"/>
+    <sheet name="k-means(num_plasma)" sheetId="7" r:id="rId6"/>
+    <sheet name="fftss" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="64">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -269,15 +270,27 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>execution time (100000, iteration = 1000, clusters = 100, procs = 4)</t>
+    <t>c-0.1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>execution time (100000, iteration = 1000, clusters = 1000, procs = 16)</t>
+    <t>compress ratio (iteration = 1000, clusters = 100)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>c-0.1</t>
+    <t>execution time (2366316, iteration = 1000, clusters = 100, procs = 4)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>execution time (2366316, iteration = 1000, clusters = 1000, procs = 16)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>execution time (4386200, iteration = 1000, clusters = 100, procs = 4)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>execution time (4386200, iteration = 1000, clusters = 1000, procs = 16)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -15385,7 +15398,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G26"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15488,7 +15501,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -15682,15 +15695,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D4BC53-861A-4F44-A625-5CE21B6F2D0F}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -15716,7 +15729,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -15795,7 +15808,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -15843,7 +15856,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -15937,6 +15950,264 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF5ED9B-4ACE-2440-B1F1-17CD48003D82}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3">
+        <v>2206.6678849999998</v>
+      </c>
+      <c r="C3">
+        <v>2159.9150559999998</v>
+      </c>
+      <c r="D3">
+        <v>2220.9988400000002</v>
+      </c>
+      <c r="E3">
+        <v>2105.8497699999998</v>
+      </c>
+      <c r="F3">
+        <v>2205.4593639999998</v>
+      </c>
+      <c r="G3">
+        <v>2172.3178710000002</v>
+      </c>
+      <c r="H3">
+        <v>2165.6020990000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D6">
+        <v>1E-4</v>
+      </c>
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="E7">
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="F7">
+        <v>1.8320000000000001E-3</v>
+      </c>
+      <c r="G7">
+        <v>1.8320000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12">
+        <v>1.0000180000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.0004420000000001</v>
+      </c>
+      <c r="D12">
+        <v>1.115305</v>
+      </c>
+      <c r="E12">
+        <v>1.7523679999999999</v>
+      </c>
+      <c r="F12">
+        <v>6.6116710000000003</v>
+      </c>
+      <c r="G12">
+        <v>6.6116710000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C20">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D20">
+        <v>1E-4</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20">
+        <v>0.01</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C25">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D25">
+        <v>1E-4</v>
+      </c>
+      <c r="E25">
+        <v>1E-3</v>
+      </c>
+      <c r="F25">
+        <v>0.01</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>

</xml_diff>

<commit_message>
bitwise compress for himeno
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937E6BDA-5FA5-C44F-9F38-F0826AF2DA76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AC0E9E-991C-0146-9147-B620844DEE42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="4580" windowWidth="26740" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="4000" windowWidth="26740" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ping-pong" sheetId="2" r:id="rId1"/>
@@ -22071,8 +22071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -22231,6 +22231,10 @@
       </c>
     </row>
     <row r="8" spans="1:14">
+      <c r="E8">
+        <f>E6/E4</f>
+        <v>1.8707249408900424</v>
+      </c>
       <c r="I8">
         <v>8.3371000000000001E-2</v>
       </c>
@@ -22253,6 +22257,10 @@
     <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>33</v>
+      </c>
+      <c r="E9">
+        <f>E7/E5</f>
+        <v>2.9041832608296061</v>
       </c>
     </row>
     <row r="10" spans="1:14">

</xml_diff>

<commit_message>
compression pattern a, b, c, d
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A31AF6-57CE-F348-B48E-0325093E0E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DBD653-51FD-534A-8380-B7F16D756038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="3020" windowWidth="26740" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,6 @@
     <sheet name="k-means(num_plasma)" sheetId="7" r:id="rId6"/>
     <sheet name="fftss" sheetId="4" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.5" hidden="1">'ping-pong'!$H$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'ping-pong'!$H$9</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'ping-pong'!$I$7:$N$7</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'ping-pong'!$I$8:$N$8</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'ping-pong'!$I$9:$N$9</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">'ping-pong'!$H$8</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'ping-pong'!$H$9</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'ping-pong'!$I$7:$N$7</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'ping-pong'!$I$8:$N$8</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'ping-pong'!$I$9:$N$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -23266,14 +23254,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>83831</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>61823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>71129</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>660398</xdr:colOff>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>106273</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -23303,16 +23291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>608330</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>252730</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>553525</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>197925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23341,15 +23329,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>514050</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>82250</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>144406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>32775</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>274075</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>37324</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -23379,16 +23367,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23416,15 +23404,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23452,15 +23440,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>1187450</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23487,16 +23475,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25619,7 +25607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7:N9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add compress ratio sz, nolossy to kmeans
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78128612-F208-E942-933B-66CADB8C5D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B38E75-A6B4-084F-B445-E7B0AC4C46A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3400" windowWidth="26740" windowHeight="18400" tabRatio="736" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11760" yWindow="4460" windowWidth="26740" windowHeight="18400" tabRatio="736" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ping-pong" sheetId="2" r:id="rId1"/>
@@ -20,59 +20,10 @@
     <sheet name="k-means" sheetId="3" r:id="rId5"/>
     <sheet name="k-means(test)" sheetId="5" r:id="rId6"/>
     <sheet name="k-means(obs_info)" sheetId="6" r:id="rId7"/>
-    <sheet name="k-means(num_plasma)" sheetId="7" r:id="rId8"/>
-    <sheet name="fftss" sheetId="4" r:id="rId9"/>
+    <sheet name="obs_info(revise)" sheetId="10" r:id="rId8"/>
+    <sheet name="k-means(num_plasma)" sheetId="7" r:id="rId9"/>
+    <sheet name="fftss" sheetId="4" r:id="rId10"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'pingpong(revise)'!$A$3</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'pingpong(revise)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'pingpong(revise)'!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'pingpong(revise)'!$B$7:$F$7</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'pingpong(revise)'!$B$8:$F$8</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'himeno(revise)'!$A$3:$A$8</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'himeno(revise)'!$B$2</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'himeno(revise)'!$B$3:$B$8</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'himeno(revise)'!$C$2</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'himeno(revise)'!$C$3:$C$8</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'himeno(revise)'!$D$2</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'himeno(revise)'!$D$3:$D$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'pingpong(revise)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'himeno(revise)'!$E$2</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'himeno(revise)'!$E$3:$E$8</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'himeno(revise)'!$F$2</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'himeno(revise)'!$F$3:$F$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'pingpong(revise)'!$A$6</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'himeno(revise)'!$A$3</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'himeno(revise)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'himeno(revise)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'himeno(revise)'!$A$6</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'himeno(revise)'!$A$7</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'pingpong(revise)'!$A$7</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'himeno(revise)'!$A$8</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'himeno(revise)'!$B$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'himeno(revise)'!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'himeno(revise)'!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'himeno(revise)'!$B$5:$F$5</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">'himeno(revise)'!$B$6:$F$6</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">'himeno(revise)'!$B$7:$F$7</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">'himeno(revise)'!$B$8:$F$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'pingpong(revise)'!$A$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'pingpong(revise)'!$B$1:$F$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'pingpong(revise)'!$B$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'pingpong(revise)'!$B$4:$F$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'pingpong(revise)'!$B$5:$F$5</definedName>
-    <definedName name="_xlchart.v2.24" hidden="1">'himeno(revise)'!$A$3:$A$8</definedName>
-    <definedName name="_xlchart.v2.25" hidden="1">'himeno(revise)'!$B$2</definedName>
-    <definedName name="_xlchart.v2.26" hidden="1">'himeno(revise)'!$B$3:$B$8</definedName>
-    <definedName name="_xlchart.v2.27" hidden="1">'himeno(revise)'!$C$2</definedName>
-    <definedName name="_xlchart.v2.28" hidden="1">'himeno(revise)'!$C$3:$C$8</definedName>
-    <definedName name="_xlchart.v2.29" hidden="1">'himeno(revise)'!$D$2</definedName>
-    <definedName name="_xlchart.v2.30" hidden="1">'himeno(revise)'!$D$3:$D$8</definedName>
-    <definedName name="_xlchart.v2.31" hidden="1">'himeno(revise)'!$E$2</definedName>
-    <definedName name="_xlchart.v2.32" hidden="1">'himeno(revise)'!$E$3:$E$8</definedName>
-    <definedName name="_xlchart.v2.33" hidden="1">'himeno(revise)'!$F$2</definedName>
-    <definedName name="_xlchart.v2.34" hidden="1">'himeno(revise)'!$F$3:$F$8</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -86,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="84">
   <si>
     <t>byte</t>
     <phoneticPr fontId="1"/>
@@ -34893,6 +34844,304 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D2">
+        <v>1E-4</v>
+      </c>
+      <c r="E2">
+        <v>1E-3</v>
+      </c>
+      <c r="F2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3">
+        <f>AVERAGE(B4:B7)</f>
+        <v>6.21041825</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(C4:C7)</f>
+        <v>6.21041825</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D4:D7)</f>
+        <v>6.21041825</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(E4:E7)</f>
+        <v>6.21041825</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(F4:F7)</f>
+        <v>6.21041825</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="C4">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="D4">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="E4">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="F4">
+        <v>7.9996809999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="C5">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="D5">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="E5">
+        <v>7.9996809999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.9996809999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6">
+        <v>1.0025649999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.0025649999999999</v>
+      </c>
+      <c r="D6">
+        <v>1.0025649999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.0025649999999999</v>
+      </c>
+      <c r="F6">
+        <v>1.0025649999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7">
+        <v>7.8397459999999999</v>
+      </c>
+      <c r="C7">
+        <v>7.8397459999999999</v>
+      </c>
+      <c r="D7">
+        <v>7.8397459999999999</v>
+      </c>
+      <c r="E7">
+        <v>7.8397459999999999</v>
+      </c>
+      <c r="F7">
+        <v>7.8397459999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11">
+        <v>4.2609000000000001E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.2356</v>
+      </c>
+      <c r="D11">
+        <v>0.26866699999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.31279600000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.267152</v>
+      </c>
+      <c r="G11">
+        <v>0.26097100000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13">
+        <v>4.2609000000000001E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.27939599999999998</v>
+      </c>
+      <c r="D13">
+        <v>0.21291599999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.18334600000000001</v>
+      </c>
+      <c r="F13">
+        <v>1.553126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15">
+        <v>2.2270000000000002E-2</v>
+      </c>
+      <c r="E15">
+        <v>2.8202000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="D16">
+        <v>1.9782000000000001E-2</v>
+      </c>
+      <c r="E16">
+        <v>2.2936000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="D17">
+        <v>1.8460000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>2.4346E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="D18">
+        <v>2.6015E-2</v>
+      </c>
+      <c r="E18">
+        <v>3.0252999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="D19">
+        <f>SUM(D15:D18)</f>
+        <v>8.6527000000000007E-2</v>
+      </c>
+      <c r="E19">
+        <f>SUM(E15:E18)</f>
+        <v>0.105737</v>
+      </c>
+      <c r="F19">
+        <f>D19/E19</f>
+        <v>0.81832281982655086</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>4.2609000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>0.21291599999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>3.8682000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V15"/>
@@ -35692,8 +35941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F313FB-83AD-0442-9AB5-FB15F7618C96}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -36551,7 +36800,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:G12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
@@ -36806,6 +37055,91 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9925E5E1-8053-134A-937E-D64A5823C4EF}">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="B2">
+        <v>-6</v>
+      </c>
+      <c r="C2">
+        <v>-5</v>
+      </c>
+      <c r="D2">
+        <v>-4</v>
+      </c>
+      <c r="E2">
+        <v>-3</v>
+      </c>
+      <c r="F2">
+        <v>-2</v>
+      </c>
+      <c r="J2">
+        <v>-6</v>
+      </c>
+      <c r="K2">
+        <v>-5</v>
+      </c>
+      <c r="L2">
+        <v>-4</v>
+      </c>
+      <c r="M2">
+        <v>-3</v>
+      </c>
+      <c r="N2">
+        <v>-2</v>
+      </c>
+      <c r="R2">
+        <v>-6</v>
+      </c>
+      <c r="S2">
+        <v>-5</v>
+      </c>
+      <c r="T2">
+        <v>-4</v>
+      </c>
+      <c r="U2">
+        <v>-3</v>
+      </c>
+      <c r="V2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="F3">
+        <v>3.4551639999999999</v>
+      </c>
+      <c r="N3">
+        <v>599.73800900000003</v>
+      </c>
+      <c r="V3">
+        <v>1.7229999999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
@@ -37062,302 +37396,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C2">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="D2">
-        <v>1E-4</v>
-      </c>
-      <c r="E2">
-        <v>1E-3</v>
-      </c>
-      <c r="F2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3">
-        <f>AVERAGE(B4:B7)</f>
-        <v>6.21041825</v>
-      </c>
-      <c r="C3">
-        <f>AVERAGE(C4:C7)</f>
-        <v>6.21041825</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGE(D4:D7)</f>
-        <v>6.21041825</v>
-      </c>
-      <c r="E3">
-        <f>AVERAGE(E4:E7)</f>
-        <v>6.21041825</v>
-      </c>
-      <c r="F3">
-        <f>AVERAGE(F4:F7)</f>
-        <v>6.21041825</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="C4">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="D4">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="E4">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="F4">
-        <v>7.9996809999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="C5">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="D5">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="E5">
-        <v>7.9996809999999998</v>
-      </c>
-      <c r="F5">
-        <v>7.9996809999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6">
-        <v>1.0025649999999999</v>
-      </c>
-      <c r="C6">
-        <v>1.0025649999999999</v>
-      </c>
-      <c r="D6">
-        <v>1.0025649999999999</v>
-      </c>
-      <c r="E6">
-        <v>1.0025649999999999</v>
-      </c>
-      <c r="F6">
-        <v>1.0025649999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7">
-        <v>7.8397459999999999</v>
-      </c>
-      <c r="C7">
-        <v>7.8397459999999999</v>
-      </c>
-      <c r="D7">
-        <v>7.8397459999999999</v>
-      </c>
-      <c r="E7">
-        <v>7.8397459999999999</v>
-      </c>
-      <c r="F7">
-        <v>7.8397459999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11">
-        <v>4.2609000000000001E-2</v>
-      </c>
-      <c r="C11">
-        <v>0.2356</v>
-      </c>
-      <c r="D11">
-        <v>0.26866699999999999</v>
-      </c>
-      <c r="E11">
-        <v>0.31279600000000002</v>
-      </c>
-      <c r="F11">
-        <v>0.267152</v>
-      </c>
-      <c r="G11">
-        <v>0.26097100000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13">
-        <v>4.2609000000000001E-2</v>
-      </c>
-      <c r="C13">
-        <v>0.27939599999999998</v>
-      </c>
-      <c r="D13">
-        <v>0.21291599999999999</v>
-      </c>
-      <c r="E13">
-        <v>0.18334600000000001</v>
-      </c>
-      <c r="F13">
-        <v>1.553126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="D15">
-        <v>2.2270000000000002E-2</v>
-      </c>
-      <c r="E15">
-        <v>2.8202000000000001E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="D16">
-        <v>1.9782000000000001E-2</v>
-      </c>
-      <c r="E16">
-        <v>2.2936000000000002E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="D17">
-        <v>1.8460000000000001E-2</v>
-      </c>
-      <c r="E17">
-        <v>2.4346E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="D18">
-        <v>2.6015E-2</v>
-      </c>
-      <c r="E18">
-        <v>3.0252999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="D19">
-        <f>SUM(D15:D18)</f>
-        <v>8.6527000000000007E-2</v>
-      </c>
-      <c r="E19">
-        <f>SUM(E15:E18)</f>
-        <v>0.105737</v>
-      </c>
-      <c r="F19">
-        <f>D19/E19</f>
-        <v>0.81832281982655086</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>4.2609000000000001E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22">
-        <v>0.21291599999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23">
-        <v>3.8682000000000001E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
crop frames of pics
</commit_message>
<xml_diff>
--- a/impl/data-compression.xlsx
+++ b/impl/data-compression.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smallcat\Documents\github\data-compression\impl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smallcat/Documents/github/data-compression/impl/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DECBF1-F56A-664A-94AE-CE2EDF409E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="3996" windowWidth="26736" windowHeight="18396" tabRatio="887" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="3040" yWindow="900" windowWidth="26740" windowHeight="18400" tabRatio="887" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ping-pong" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
     <sheet name="simgrid(matrix)" sheetId="15" r:id="rId14"/>
     <sheet name="simgrid(reversal)" sheetId="16" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -400,7 +401,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -1737,12 +1738,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2157,7 +2153,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2409,12 +2404,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -3015,12 +3005,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -4807,12 +4792,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -10188,12 +10168,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -10796,12 +10771,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -11214,12 +11184,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -11745,7 +11710,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13369,12 +13333,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -13975,12 +13934,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -14390,12 +14344,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -16033,12 +15982,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -16639,12 +16583,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -17405,12 +17344,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -18011,12 +17945,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -18777,12 +18706,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -19837,12 +19761,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -22390,12 +22309,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -22919,12 +22833,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -45139,7 +45048,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -45169,7 +45084,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="グラフ 3"/>
+        <xdr:cNvPr id="4" name="グラフ 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -45204,7 +45125,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -45236,7 +45163,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -45273,7 +45206,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1"/>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -45305,7 +45244,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2"/>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -51711,18 +51656,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.796875" customWidth="1"/>
-    <col min="2" max="2" width="9.296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -52124,14 +52069,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:V11"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="159" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
@@ -52509,14 +52454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -52807,14 +52752,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A21:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
@@ -52866,14 +52811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -53044,23 +52989,23 @@
         <v>73</v>
       </c>
       <c r="P5" s="1">
-        <f>P9/P$8</f>
+        <f t="shared" ref="P5:T6" si="0">P9/P$8</f>
         <v>1.1857481776264183</v>
       </c>
       <c r="Q5" s="1">
-        <f>Q9/Q$8</f>
+        <f t="shared" si="0"/>
         <v>1.1116606399193882</v>
       </c>
       <c r="R5" s="1">
-        <f>R9/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.93185630193684998</v>
       </c>
       <c r="S5" s="1">
-        <f>S9/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.76514180394257691</v>
       </c>
       <c r="T5" s="1">
-        <f>T9/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.70089476470175582</v>
       </c>
     </row>
@@ -53087,23 +53032,23 @@
         <v>74</v>
       </c>
       <c r="P6" s="1">
-        <f>P10/P$8</f>
+        <f t="shared" si="0"/>
         <v>0.54626883757118905</v>
       </c>
       <c r="Q6" s="1">
-        <f>Q10/Q$8</f>
+        <f t="shared" si="0"/>
         <v>0.45438804599460464</v>
       </c>
       <c r="R6" s="1">
-        <f>R10/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.34298888399946431</v>
       </c>
       <c r="S6" s="1">
-        <f>S10/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.27913693152467139</v>
       </c>
       <c r="T6" s="1">
-        <f>T10/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.13414232052091504</v>
       </c>
     </row>
@@ -53481,14 +53426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -53659,23 +53604,23 @@
         <v>73</v>
       </c>
       <c r="P5" s="1">
-        <f>P9/P$8</f>
+        <f t="shared" ref="P5:T6" si="0">P9/P$8</f>
         <v>0.99977326240516262</v>
       </c>
       <c r="Q5" s="1">
-        <f>Q9/Q$8</f>
+        <f t="shared" si="0"/>
         <v>0.96331211301997022</v>
       </c>
       <c r="R5" s="1">
-        <f>R9/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.87642801081363908</v>
       </c>
       <c r="S5" s="1">
-        <f>S9/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.79263626057382053</v>
       </c>
       <c r="T5" s="1">
-        <f>T9/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.72626667829423563</v>
       </c>
     </row>
@@ -53702,23 +53647,23 @@
         <v>74</v>
       </c>
       <c r="P6" s="1">
-        <f>P10/P$8</f>
+        <f t="shared" si="0"/>
         <v>0.42863259788959623</v>
       </c>
       <c r="Q6" s="1">
-        <f>Q10/Q$8</f>
+        <f t="shared" si="0"/>
         <v>0.35024766721897621</v>
       </c>
       <c r="R6" s="1">
-        <f>R10/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.25520886020755212</v>
       </c>
       <c r="S6" s="1">
-        <f>S10/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.18032528124182437</v>
       </c>
       <c r="T6" s="1">
-        <f>T10/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.11155402459230834</v>
       </c>
     </row>
@@ -54096,14 +54041,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -54274,23 +54219,23 @@
         <v>73</v>
       </c>
       <c r="P5" s="1">
-        <f>P9/P$8</f>
+        <f t="shared" ref="P5:T6" si="0">P9/P$8</f>
         <v>0.96960844161506932</v>
       </c>
       <c r="Q5" s="1">
-        <f>Q9/Q$8</f>
+        <f t="shared" si="0"/>
         <v>0.93607743960931356</v>
       </c>
       <c r="R5" s="1">
-        <f>R9/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.85611406645155663</v>
       </c>
       <c r="S5" s="1">
-        <f>S9/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.78124705677160544</v>
       </c>
       <c r="T5" s="1">
-        <f>T9/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.71676550100287784</v>
       </c>
     </row>
@@ -54317,23 +54262,23 @@
         <v>74</v>
       </c>
       <c r="P6" s="1">
-        <f>P10/P$8</f>
+        <f t="shared" si="0"/>
         <v>0.41503706287607911</v>
       </c>
       <c r="Q6" s="1">
-        <f>Q10/Q$8</f>
+        <f t="shared" si="0"/>
         <v>0.33911049097409957</v>
       </c>
       <c r="R6" s="1">
-        <f>R10/R$8</f>
+        <f t="shared" si="0"/>
         <v>0.24705241126711433</v>
       </c>
       <c r="S6" s="1">
-        <f>S10/S$8</f>
+        <f t="shared" si="0"/>
         <v>0.17038719804656838</v>
       </c>
       <c r="T6" s="1">
-        <f>T10/T$8</f>
+        <f t="shared" si="0"/>
         <v>0.11154355978023894</v>
       </c>
     </row>
@@ -54711,16 +54656,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" zoomScale="118" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:V5"/>
+    <sheetView topLeftCell="H22" zoomScale="118" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.19921875" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -55197,16 +55142,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.69921875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -55509,14 +55454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="99" workbookViewId="0">
       <selection activeCell="I4" sqref="I4:N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:6">
       <c r="B2">
@@ -55668,14 +55613,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22:G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -56068,14 +56013,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -56367,14 +56312,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -56626,14 +56571,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
@@ -57012,14 +56957,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">

</xml_diff>